<commit_message>
Added new Zn to invatory
</commit_message>
<xml_diff>
--- a/Charge 09 - T07.xlsx
+++ b/Charge 09 - T07.xlsx
@@ -4838,7 +4838,7 @@
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="172" t="str">
         <f>"Actual  " &amp; 'Charge 09'!I3</f>
-        <v>Actual  Mg92.9Ca7.1</v>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="173"/>
       <c r="C3" s="173"/>
@@ -4902,11 +4902,11 @@
       </c>
       <c r="B6" s="105">
         <f>IF('Charge 09'!B14=0, "-", 'Charge 09'!B14)</f>
-        <v>4.6310000000000002</v>
-      </c>
-      <c r="C6" s="137" t="str">
+        <v>5.423</v>
+      </c>
+      <c r="C6" s="137">
         <f>IF('Charge 09'!E14=0,"-",'Charge 09'!E14)</f>
-        <v>-</v>
+        <v>16.215</v>
       </c>
       <c r="D6" s="137">
         <f>IF('Charge 09'!H14=0, "-", 'Charge 09'!H14)</f>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -4935,11 +4935,11 @@
       </c>
       <c r="B7" s="108">
         <f>IF('Charge 09'!B15=0, "-", 'Charge 09'!B15)</f>
-        <v>5.423</v>
-      </c>
-      <c r="C7" s="107" t="str">
+        <v>7.65</v>
+      </c>
+      <c r="C7" s="107">
         <f>IF('Charge 09'!E15=0,"-",'Charge 09'!E15)</f>
-        <v>-</v>
+        <v>17.77</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>IF('Charge 09'!H15=0, "-", 'Charge 09'!H15)</f>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -4968,11 +4968,11 @@
       </c>
       <c r="B8" s="108">
         <f>IF('Charge 09'!B16=0, "-", 'Charge 09'!B16)</f>
-        <v>6.4029999999999996</v>
-      </c>
-      <c r="C8" s="107" t="str">
+        <v>8.8849999999999998</v>
+      </c>
+      <c r="C8" s="107">
         <f>IF('Charge 09'!E16=0,"-",'Charge 09'!E16)</f>
-        <v>-</v>
+        <v>18.448</v>
       </c>
       <c r="D8" s="107" t="str">
         <f>IF('Charge 09'!H16=0, "-", 'Charge 09'!H16)</f>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="B9" s="108">
         <f>IF('Charge 09'!B17=0, "-", 'Charge 09'!B17)</f>
-        <v>7.2930000000000001</v>
+        <v>9.077</v>
       </c>
       <c r="C9" s="107" t="str">
         <f>IF('Charge 09'!E17=0,"-",'Charge 09'!E17)</f>
@@ -5034,7 +5034,7 @@
       </c>
       <c r="B10" s="108">
         <f>IF('Charge 09'!B18=0, "-", 'Charge 09'!B18)</f>
-        <v>8.827</v>
+        <v>11.194000000000001</v>
       </c>
       <c r="C10" s="107" t="str">
         <f>IF('Charge 09'!E18=0,"-",'Charge 09'!E18)</f>
@@ -5065,9 +5065,9 @@
       <c r="A11" s="27">
         <v>6</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="108" t="str">
         <f>IF('Charge 09'!B19=0, "-", 'Charge 09'!B19)</f>
-        <v>9.532</v>
+        <v>-</v>
       </c>
       <c r="C11" s="107" t="str">
         <f>IF('Charge 09'!E19=0,"-",'Charge 09'!E19)</f>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5334,11 +5334,11 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>42.108999999999995</v>
+        <v>42.228999999999999</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>52.433</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>47.448999999999998</v>
+        <v>100.00200000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5392,11 +5392,11 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-0.11300000000000665</v>
+        <v>6.9999999999978968E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-52.421999999999997</v>
+        <v>1.1000000000002785E-2</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
@@ -5412,7 +5412,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-52.551000000000002</v>
+        <v>2.0000000000095497E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5438,7 +5438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg92.9Ca7.1</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5614,19 +5614,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>42.108999999999995</v>
+        <v>42.228999999999999</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0.88745811292124166</v>
+        <v>0.42228155436891257</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>3.6513396952118561E-2</v>
+        <v>1.7374266791561923E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0.92858681141228538</v>
+        <v>0.6500893588995702</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5711,19 +5711,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
+        <v>52.433</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0</v>
+        <v>0.52431951360972773</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
+        <v>8.0193250987997868E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0</v>
+        <v>0.30005743406783031</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5812,15 +5812,15 @@
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>0.11254188707875824</v>
+        <v>5.3398932021359563E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>2.8080714376655081E-3</v>
+        <v>1.3323751689545277E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>7.1413188587714602E-2</v>
+        <v>4.9853207032599538E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6096,7 +6096,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>47.448999999999998</v>
+        <v>100.00200000000001</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>3.9321468389784071E-2</v>
+        <v>2.6725967059316236E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>4.6310000000000002</v>
+        <v>5.423</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6265,7 +6265,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>16.215</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6310,7 +6310,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>5.423</v>
+        <v>7.65</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6318,7 +6318,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>17.77</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>6.4029999999999996</v>
+        <v>8.8849999999999998</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="E16" s="106">
         <f>B!C4</f>
-        <v>0</v>
+        <v>18.448</v>
       </c>
       <c r="F16" s="107"/>
       <c r="G16" s="126">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="B17" s="106">
         <f>A!C5</f>
-        <v>7.2930000000000001</v>
+        <v>9.077</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="126">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="B18" s="106">
         <f>A!C6</f>
-        <v>8.827</v>
+        <v>11.194000000000001</v>
       </c>
       <c r="C18" s="107"/>
       <c r="D18" s="126">
@@ -6524,7 +6524,7 @@
       </c>
       <c r="B19" s="106">
         <f>A!C7</f>
-        <v>9.532</v>
+        <v>0</v>
       </c>
       <c r="C19" s="107"/>
       <c r="D19" s="126">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>42.108999999999995</v>
+        <v>42.228999999999999</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -6979,7 +6979,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>52.433</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7012,7 +7012,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-0.11300000000000665</v>
+        <v>6.9999999999978968E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7020,7 +7020,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-52.421999999999997</v>
+        <v>1.1000000000002785E-2</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -8439,18 +8439,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="166">
-        <v>4.6310000000000002</v>
+        <v>5.423</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>4.6310000000000002</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>5.423</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>42.108999999999995</v>
+        <v>42.228999999999999</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
@@ -8462,14 +8462,14 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>5.423</v>
+        <v>7.65</v>
       </c>
       <c r="B3" s="125">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>5.423</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>7.65</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8477,19 +8477,19 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>42.108999999999995</v>
+        <v>42.228999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>6.4029999999999996</v>
+        <v>8.8849999999999998</v>
       </c>
       <c r="B4" s="125">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>6.4029999999999996</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>8.8849999999999998</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8497,150 +8497,150 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-0.11300000000000665</v>
+        <v>6.9999999999978968E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>7.2930000000000001</v>
+        <v>9.077</v>
       </c>
       <c r="B5" s="125">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>7.2930000000000001</v>
+        <f>IF(A5=0, 0, A5*B5)</f>
+        <v>9.077</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>8.827</v>
+        <v>11.194000000000001</v>
       </c>
       <c r="B6" s="125">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>8.827</v>
+        <f>IF(A6=0, 0, A6*B6)</f>
+        <v>11.194000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>9.532</v>
+        <v>4.6310000000000002</v>
       </c>
       <c r="B7" s="125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>9.532</v>
+        <f>IF(A7=0, 0, A7*B7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="166">
-        <v>4.7190000000000003</v>
+        <v>6.4029999999999996</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166">
-        <v>7.2080000000000002</v>
+        <v>7.2930000000000001</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="166">
-        <v>7.6059999999999999</v>
+        <v>8.827</v>
       </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(A10=0, 0, A10*B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="166">
-        <v>7.65</v>
+        <v>9.532</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(A11=0, 0, A11*B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="166">
-        <v>8.0250000000000004</v>
+        <v>4.7190000000000003</v>
       </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(A12=0, 0, A12*B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="166">
-        <v>8.6</v>
+        <v>7.2080000000000002</v>
       </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(A13=0, 0, A13*B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="166">
-        <v>8.8849999999999998</v>
+        <v>7.6059999999999999</v>
       </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>IF(A14=0, 0, A14*B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="166">
-        <v>9.077</v>
+        <v>8.0250000000000004</v>
       </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>IF(A15=0, 0, A15*B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="166">
-        <v>11.194000000000001</v>
+        <v>8.6</v>
       </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>IF(A16=0, 0, A16*B16)</f>
         <v>0</v>
       </c>
     </row>
@@ -8652,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>IF(A17=0, 0, A17*B17)</f>
         <v>0</v>
       </c>
     </row>
@@ -8662,7 +8662,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>IF(A18=0, 0, A18*B18)</f>
         <v>0</v>
       </c>
     </row>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f>IF(A19=0, 0, A19*B19)</f>
         <v>0</v>
       </c>
     </row>
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>IF(A20=0, 0, A20*B20)</f>
         <v>0</v>
       </c>
     </row>
@@ -8692,7 +8692,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>IF(A21=0, 0, A21*B21)</f>
         <v>0</v>
       </c>
     </row>
@@ -8702,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>IF(A22=0, 0, A22*B22)</f>
         <v>0</v>
       </c>
     </row>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f>IF(A23=0, 0, A23*B23)</f>
         <v>0</v>
       </c>
     </row>
@@ -8722,7 +8722,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f>IF(A24=0, 0, A24*B24)</f>
         <v>0</v>
       </c>
     </row>
@@ -8732,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f>IF(A25=0, 0, A25*B25)</f>
         <v>0</v>
       </c>
     </row>
@@ -8742,7 +8742,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f>IF(A26=0, 0, A26*B26)</f>
         <v>0</v>
       </c>
     </row>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f>IF(A27=0, 0, A27*B27)</f>
         <v>0</v>
       </c>
     </row>
@@ -8762,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f>IF(A28=0, 0, A28*B28)</f>
         <v>0</v>
       </c>
     </row>
@@ -8772,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
@@ -8782,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
@@ -8792,7 +8792,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -8802,7 +8802,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -8812,7 +8812,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -8822,7 +8822,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8832,7 +8832,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -8842,7 +8842,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -8852,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -8862,7 +8862,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8872,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -8892,7 +8892,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -8902,7 +8902,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -8912,7 +8912,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -8922,7 +8922,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -8932,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -8942,7 +8942,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -8952,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -8962,7 +8962,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -8972,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -8982,7 +8982,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -8992,7 +8992,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
@@ -9016,7 +9016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9051,18 +9051,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>12.38</v>
+        <v>16.215</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f>IF(A2=0, 0, A2*B2)</f>
+        <v>16.215</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>52.433</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
@@ -9074,321 +9074,363 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>12.622</v>
+        <v>17.77</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(A3=0, 0, A3*B3)</f>
+        <v>17.77</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>52.433</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>13.234</v>
+        <v>18.448</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(A4=0, 0, A4*B4)</f>
+        <v>18.448</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-52.421999999999997</v>
+        <v>1.1000000000002785E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>14.38</v>
+        <v>7.9569999999999999</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>IF(A5=0, 0, A5*B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>17.77</v>
+        <v>9.3650000000000002</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>19.841999999999999</v>
+        <v>9.8140000000000001</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(A7=0, 0, A7*B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>20.332000000000001</v>
+        <v>10.753</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(A8=0, 0, A8*B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>20.411999999999999</v>
+        <v>11.766</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(A9=0, 0, A9*B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="125">
+        <v>12.38</v>
+      </c>
+      <c r="B10" s="125">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>IF(A10=0, 0, A10*B10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="125">
+        <v>12.622</v>
+      </c>
+      <c r="B11" s="125">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>IF(A11=0, 0, A11*B11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="125">
+        <v>12.919</v>
+      </c>
+      <c r="B12" s="125">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>IF(A12=0, 0, A12*B12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="125">
+        <v>13.013999999999999</v>
+      </c>
+      <c r="B13" s="125">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>IF(A13=0, 0, A13*B13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="125">
+        <v>13.234</v>
+      </c>
+      <c r="B14" s="125">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>IF(A14=0, 0, A14*B14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="125">
+        <v>13.683</v>
+      </c>
+      <c r="B15" s="125">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>IF(A15=0, 0, A15*B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="125">
+        <v>14.233000000000001</v>
+      </c>
+      <c r="B16" s="125">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>IF(A16=0, 0, A16*B16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="125">
+        <v>14.38</v>
+      </c>
+      <c r="B17" s="125">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>IF(A17=0, 0, A17*B17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="125">
+        <v>14.795999999999999</v>
+      </c>
+      <c r="B18" s="125">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>IF(A18=0, 0, A18*B18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="125">
+        <v>15.151</v>
+      </c>
+      <c r="B19" s="125">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>IF(A19=0, 0, A19*B19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="125">
+        <v>15.32</v>
+      </c>
+      <c r="B20" s="125">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>IF(A20=0, 0, A20*B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="125">
+        <v>16.3</v>
+      </c>
+      <c r="B21" s="125">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>IF(A21=0, 0, A21*B21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="125">
+        <v>17.824000000000002</v>
+      </c>
+      <c r="B22" s="125">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>IF(A22=0, 0, A22*B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="125">
+        <v>19.215</v>
+      </c>
+      <c r="B23" s="125">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>IF(A23=0, 0, A23*B23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="125">
+        <v>19.731999999999999</v>
+      </c>
+      <c r="B24" s="125">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>IF(A24=0, 0, A24*B24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="125">
+        <v>19.754000000000001</v>
+      </c>
+      <c r="B25" s="125">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>IF(A25=0, 0, A25*B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="125">
+        <v>19.841999999999999</v>
+      </c>
+      <c r="B26" s="125">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>IF(A26=0, 0, A26*B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="125">
+        <v>20.332000000000001</v>
+      </c>
+      <c r="B27" s="125">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>IF(A27=0, 0, A27*B27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="125">
+        <v>20.411999999999999</v>
+      </c>
+      <c r="B28" s="125">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>IF(A28=0, 0, A28*B28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="125">
         <v>20.777000000000001</v>
       </c>
-      <c r="B10" s="125">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="125">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="125">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="125">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
-      <c r="B14" s="125">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
-      <c r="B15" s="125">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
-      <c r="B16" s="125">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
-      <c r="B17" s="125">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
-      <c r="B18" s="125">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
-      <c r="B19" s="125">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
-      <c r="B20" s="125">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="125"/>
-      <c r="B21" s="125">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="125">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="125"/>
-      <c r="B23" s="125">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="125"/>
-      <c r="B24" s="125">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
-      <c r="B25" s="125">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="125"/>
-      <c r="B26" s="125">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="125"/>
-      <c r="B27" s="125">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="125">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="125"/>
       <c r="B29" s="125">
         <v>0</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f>IF(A29=0, 0, A29*B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
+      <c r="A30" s="125">
+        <v>21.151</v>
+      </c>
       <c r="B30" s="125">
         <v>0</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f>IF(A30=0, 0, A30*B30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
+      <c r="A31" s="125">
+        <v>21.282</v>
+      </c>
       <c r="B31" s="125">
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f>IF(A31=0, 0, A31*B31)</f>
         <v>0</v>
       </c>
     </row>
@@ -9398,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f>IF(A32=0, 0, A32*B32)</f>
         <v>0</v>
       </c>
     </row>
@@ -9408,7 +9450,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f>IF(A33=0, 0, A33*B33)</f>
         <v>0</v>
       </c>
     </row>
@@ -9418,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
+        <f>IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9428,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>IF(A35=0, 0, A35*B35)</f>
         <v>0</v>
       </c>
     </row>
@@ -9438,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>IF(A36=0, 0, A36*B36)</f>
         <v>0</v>
       </c>
     </row>
@@ -9448,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f>IF(A37=0, 0, A37*B37)</f>
         <v>0</v>
       </c>
     </row>
@@ -9458,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f>IF(A38=0, 0, A38*B38)</f>
         <v>0</v>
       </c>
     </row>
@@ -9468,7 +9510,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f>IF(A39=0, 0, A39*B39)</f>
         <v>0</v>
       </c>
     </row>
@@ -9478,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f>IF(A40=0, 0, A40*B40)</f>
         <v>0</v>
       </c>
     </row>
@@ -9488,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f>IF(A41=0, 0, A41*B41)</f>
         <v>0</v>
       </c>
     </row>
@@ -9498,7 +9540,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f>IF(A42=0, 0, A42*B42)</f>
         <v>0</v>
       </c>
     </row>
@@ -9508,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f>IF(A43=0, 0, A43*B43)</f>
         <v>0</v>
       </c>
     </row>
@@ -9518,7 +9560,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f>IF(A44=0, 0, A44*B44)</f>
         <v>0</v>
       </c>
     </row>
@@ -9528,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f>IF(A45=0, 0, A45*B45)</f>
         <v>0</v>
       </c>
     </row>
@@ -9538,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f>IF(A46=0, 0, A46*B46)</f>
         <v>0</v>
       </c>
     </row>
@@ -9548,7 +9590,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f>IF(A47=0, 0, A47*B47)</f>
         <v>0</v>
       </c>
     </row>
@@ -9558,7 +9600,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f>IF(A48=0, 0, A48*B48)</f>
         <v>0</v>
       </c>
     </row>
@@ -9568,7 +9610,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f>IF(A49=0, 0, A49*B49)</f>
         <v>0</v>
       </c>
     </row>
@@ -9578,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f>IF(A50=0, 0, A50*B50)</f>
         <v>0</v>
       </c>
     </row>
@@ -9588,14 +9630,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f>IF(A51=0, 0, A51*B51)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
09, not sure what changed
</commit_message>
<xml_diff>
--- a/Charge 09 - T07.xlsx
+++ b/Charge 09 - T07.xlsx
@@ -4906,11 +4906,11 @@
       </c>
       <c r="C6" s="137">
         <f>IF('Charge 09'!E14=0,"-",'Charge 09'!E14)</f>
-        <v>16.215</v>
+        <v>16.178999999999998</v>
       </c>
       <c r="D6" s="137">
         <f>IF('Charge 09'!H14=0, "-", 'Charge 09'!H14)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="E6" s="137" t="str">
         <f>IF('Charge 09'!K14=0, "-", 'Charge 09'!K14)</f>
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>52.433</v>
+        <v>52.396999999999998</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>100.00200000000001</v>
+        <v>100.01400000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5396,11 +5396,11 @@
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>1.1000000000002785E-2</v>
+        <v>-2.4999999999998579E-2</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
-        <v>-1.6000000000000014E-2</v>
+        <v>3.2000000000000028E-2</v>
       </c>
       <c r="E23" s="140">
         <f t="shared" si="0"/>
@@ -5412,7 +5412,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>2.0000000000095497E-3</v>
+        <v>1.4000000000010004E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5438,7 +5438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5618,15 +5618,15 @@
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0.42228155436891257</v>
+        <v>0.42223088767572536</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>1.7374266791561923E-2</v>
+        <v>1.737218217139376E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0.6500893588995702</v>
+        <v>0.6499320089762185</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5711,19 +5711,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>52.433</v>
+        <v>52.396999999999998</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0.52431951360972773</v>
+        <v>0.52389665446837441</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>8.0193250987997868E-3</v>
+        <v>8.012857582643149E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0.30005743406783031</v>
+        <v>0.29977884038673813</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5808,19 +5808,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>5.3398932021359563E-2</v>
+        <v>5.3872457855900169E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>1.3323751689545277E-3</v>
+        <v>1.3441902753605511E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>4.9853207032599538E-2</v>
+        <v>5.0289150637043332E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6096,15 +6096,15 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>100.00200000000001</v>
+        <v>100.01400000000001</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.6725967059316236E-2</v>
+        <v>2.672923002939746E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
@@ -6243,7 +6243,7 @@
         <v>93</v>
       </c>
       <c r="Q13" s="39">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="R13" s="10" t="s">
         <v>104</v>
@@ -6265,7 +6265,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>16.215</v>
+        <v>16.178999999999998</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6979,7 +6979,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>52.433</v>
+        <v>52.396999999999998</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -6987,7 +6987,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7020,7 +7020,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>1.1000000000002785E-2</v>
+        <v>-2.4999999999998579E-2</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="H30" s="113">
         <f>H29-$F$6</f>
-        <v>-1.6000000000000014E-2</v>
+        <v>3.2000000000000028E-2</v>
       </c>
       <c r="I30" s="114"/>
       <c r="J30" s="112" t="s">
@@ -8445,7 +8445,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
         <v>5.423</v>
       </c>
       <c r="D2" s="1">
@@ -8468,7 +8468,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>7.65</v>
       </c>
       <c r="D3" s="1"/>
@@ -8488,7 +8488,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>8.8849999999999998</v>
       </c>
       <c r="D4" s="1"/>
@@ -8508,7 +8508,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>9.077</v>
       </c>
     </row>
@@ -8520,7 +8520,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>11.194000000000001</v>
       </c>
     </row>
@@ -8532,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8544,7 +8544,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8556,7 +8556,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8568,7 +8568,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8592,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8604,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8616,7 +8616,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8628,7 +8628,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8640,7 +8640,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8652,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8662,7 +8662,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8692,7 +8692,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8702,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8722,7 +8722,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8732,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8742,7 +8742,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8762,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8772,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8782,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8792,7 +8792,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8802,7 +8802,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8812,7 +8812,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8822,7 +8822,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8832,7 +8832,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8842,7 +8842,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8852,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8862,7 +8862,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8872,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8882,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8892,7 +8892,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8902,7 +8902,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8912,7 +8912,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8922,7 +8922,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8932,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8942,7 +8942,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8952,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8962,7 +8962,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8972,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8982,7 +8982,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8992,7 +8992,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9016,7 +9016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9051,18 +9051,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>16.215</v>
+        <v>16.178999999999998</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>16.215</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>16.178999999999998</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>52.433</v>
+        <v>52.396999999999998</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
@@ -9080,7 +9080,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
+        <f t="shared" si="0"/>
         <v>17.77</v>
       </c>
       <c r="E3" s="50" t="s">
@@ -9088,7 +9088,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>52.433</v>
+        <v>52.396999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9099,7 +9099,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>18.448</v>
       </c>
       <c r="E4" s="50" t="s">
@@ -9107,7 +9107,7 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>1.1000000000002785E-2</v>
+        <v>-2.4999999999998579E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9118,7 +9118,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9130,7 +9130,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9142,7 +9142,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9154,7 +9154,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9166,7 +9166,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9178,7 +9178,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9190,7 +9190,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9202,7 +9202,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9214,7 +9214,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9226,7 +9226,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9238,7 +9238,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9250,7 +9250,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9262,7 +9262,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9274,7 +9274,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9286,7 +9286,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9298,7 +9298,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9310,7 +9310,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9322,7 +9322,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9334,7 +9334,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9346,7 +9346,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9358,7 +9358,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9370,7 +9370,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9382,7 +9382,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9394,7 +9394,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9406,7 +9406,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9418,7 +9418,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9430,7 +9430,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9440,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9450,7 +9450,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9460,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9470,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9480,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9490,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9500,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9510,7 +9510,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9520,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9530,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9540,7 +9540,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9550,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9560,7 +9560,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9570,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9580,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9590,7 +9590,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9600,7 +9600,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9610,7 +9610,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9630,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9689,18 +9689,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
@@ -9724,7 +9724,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>5.34</v>
+        <v>5.3879999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9741,7 +9741,7 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-1.6000000000000014E-2</v>
+        <v>3.2000000000000028E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>